<commit_message>
Actialización script ancho equivalente
</commit_message>
<xml_diff>
--- a/Data/parametros_estelares.xlsx
+++ b/Data/parametros_estelares.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucia\Documents\Semestre 8 y9\Trabajo grado\Tesis_Estrellas_binarias\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E868D23-854C-4102-AC35-6C9F728BA4CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CDF6A8-C1A6-4B18-8459-C67662122D42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A0C05462-B58C-4615-BC93-4B5E13F8D899}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A0C05462-B58C-4615-BC93-4B5E13F8D899}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Periodo</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>yo</t>
+  </si>
+  <si>
+    <t>Eclipses fechas</t>
   </si>
 </sst>
 </file>
@@ -138,7 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -146,6 +149,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -461,19 +465,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B5F1EB-4E96-4D8E-A6C3-08F4AB0CFD19}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="10" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:10">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -487,7 +492,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -500,8 +505,11 @@
       <c r="E2">
         <v>4.1000000000000002E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -511,8 +519,11 @@
       <c r="E3">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="J3" s="3">
+        <v>43770</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -522,8 +533,11 @@
       <c r="E4">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="J4" s="3">
+        <v>42795</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -533,8 +547,11 @@
       <c r="E5">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="J5" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -542,7 +559,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -569,7 +586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF1C061-5AFB-4B32-A4CD-6434DA7B076F}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
pruebas de medición del ancho equivalente
</commit_message>
<xml_diff>
--- a/Data/parametros_estelares.xlsx
+++ b/Data/parametros_estelares.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucia\Documents\Semestre 8 y9\Trabajo grado\Tesis_Estrellas_binarias\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CDF6A8-C1A6-4B18-8459-C67662122D42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D10AFF5-2ECE-449A-97A2-5B96741A6279}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A0C05462-B58C-4615-BC93-4B5E13F8D899}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A0C05462-B58C-4615-BC93-4B5E13F8D899}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B5F1EB-4E96-4D8E-A6C3-08F4AB0CFD19}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -584,10 +584,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF1C061-5AFB-4B32-A4CD-6434DA7B076F}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -597,7 +597,7 @@
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -614,7 +614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -633,8 +633,11 @@
       <c r="F2">
         <v>4134</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -653,8 +656,11 @@
       <c r="F3">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -673,8 +679,11 @@
       <c r="F4">
         <v>-0.02</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -687,8 +696,11 @@
       <c r="F5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -701,8 +713,11 @@
       <c r="F6">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>12</v>
       </c>

</xml_diff>